<commit_message>
tb and staph testing
</commit_message>
<xml_diff>
--- a/indigoData/identifiers_match_tb.xlsx
+++ b/indigoData/identifiers_match_tb.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Systems Bio Research\indigo\Tuberculosis Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Systems Bio Research\indigo\indigoData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDE8D82-2AED-4EE8-86EA-5207824BE773}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CF6B60-150F-4D74-B126-C504CFFEB54B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14380" yWindow="7090" windowWidth="7500" windowHeight="6000" xr2:uid="{629EE73C-0C61-40C0-9AA6-A1E6E60449C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{629EE73C-0C61-40C0-9AA6-A1E6E60449C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD819FC-7FE2-41B8-904F-EBD6C5CEA702}">
   <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1443,71 +1443,71 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="B76" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>38</v>
+        <v>118</v>
       </c>
       <c r="B77" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>136</v>
+        <v>38</v>
       </c>
       <c r="B78" t="s">
-        <v>137</v>
+        <v>39</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="B79" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B80" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B81" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B82" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B83" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B84" t="s">
         <v>120</v>
@@ -1515,15 +1515,15 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B85" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="B86" t="s">
         <v>41</v>
@@ -1531,15 +1531,15 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>138</v>
+        <v>40</v>
       </c>
       <c r="B87" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>42</v>
+        <v>138</v>
       </c>
       <c r="B88" t="s">
         <v>43</v>
@@ -1547,7 +1547,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>128</v>
+        <v>42</v>
       </c>
       <c r="B89" t="s">
         <v>43</v>
@@ -1555,14 +1555,14 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="B90" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B89">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B90">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>